<commit_message>
added color selector textbox
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/97a86547de9b44dc/Documents/Proyectos 2024/Ticket numerator/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="32" documentId="11_F25DC773A252ABDACC1048B481185F8C5BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68BF4778-1C7A-4765-8379-114A9CD1A82C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,22 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="3">
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +350,280 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:A33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>